<commit_message>
Just got the Breach Data table working using the Responsive extension.   This allows us to drill down into the "Web.Description"
</commit_message>
<xml_diff>
--- a/LIfecycleManagement/data/ProfileAndPersona.xlsx
+++ b/LIfecycleManagement/data/ProfileAndPersona.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2180" windowWidth="27360" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DevProfile" sheetId="1" r:id="rId1"/>
+    <sheet name="UserPersona" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>DeviceProfile</t>
   </si>
@@ -66,6 +67,39 @@
   </si>
   <si>
     <t>In Patient Registration and Scheduling</t>
+  </si>
+  <si>
+    <t>AMBEXRM01</t>
+  </si>
+  <si>
+    <t>Ambulatory Exam Room</t>
+  </si>
+  <si>
+    <t>Includes Thin Client, 24" Monitor with Keyboard, Mouse, proximity card reader, biometric scanner</t>
+  </si>
+  <si>
+    <t>Includes PC, 24" Monitor with Keyboard, Mouse, Esignature Pad</t>
+  </si>
+  <si>
+    <t>ROV01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Epic Rover </t>
+  </si>
+  <si>
+    <t>Includes</t>
+  </si>
+  <si>
+    <t>UserPersonaCode</t>
+  </si>
+  <si>
+    <t>UserPersona</t>
+  </si>
+  <si>
+    <t>IsActive</t>
+  </si>
+  <si>
+    <t>Associated Roles</t>
   </si>
 </sst>
 </file>
@@ -380,20 +414,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="36.83203125" customWidth="1"/>
+    <col min="2" max="5" width="27.1640625" customWidth="1"/>
+    <col min="6" max="6" width="36.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -407,10 +441,13 @@
         <v>11</v>
       </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -423,11 +460,14 @@
       <c r="D2" t="b">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -440,11 +480,14 @@
       <c r="D3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -457,8 +500,14 @@
       <c r="D4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -470,6 +519,79 @@
       </c>
       <c r="D5" t="b">
         <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>